<commit_message>
260123 Insident and comment table create. make the ERD
</commit_message>
<xml_diff>
--- a/db/DataBaseCol.xlsx
+++ b/db/DataBaseCol.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\TeamProjectStraffic_\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\SAP_Straffic260119\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A79B49-797B-455C-95D2-07348A4D438E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0FC447-C10E-4206-8C8F-09A15A7A56EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="15720" xr2:uid="{008F3ED9-E954-48A9-9E03-D39CBFFCB847}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{008F3ED9-E954-48A9-9E03-D39CBFFCB847}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="102">
   <si>
     <t>DB</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -294,6 +294,122 @@
   </si>
   <si>
     <t>권한(1: Master 2: 운영자 3: 대기 4: 비활성화)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>insident</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록일자 Default Current_Timestamp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>완료일자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Insident ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Insident 제목</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인시던트 발생 호선명</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인시던트 발생 역ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인시던트 발생 역 이름</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인시던트 발생 내용</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인시던트 상태 (1:오픈 2:해결중 3:완료 4:비활성화)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>작성자 이름</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>insident_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>insident_title</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>insident_line_name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">insident_station_id </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>insident_station_name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>insident_content</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>insident_status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>create_at</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>complete_at</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>insident_comment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>작성자 ID ( FK storage.user(user_id) )</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글 내용</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인시던트 ID ( FK storage.insident(insident_id) )</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글 ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment_content</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -339,7 +455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -362,6 +478,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -371,7 +524,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -379,6 +532,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -696,20 +858,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A039B4-B4EC-499B-B846-66B839DA3680}">
-  <dimension ref="B2:F45"/>
+  <dimension ref="B2:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="14.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.69921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.4">
@@ -1288,8 +1450,226 @@
         <v>72</v>
       </c>
     </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B46" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B47" s="4"/>
+      <c r="C47" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B48" s="4"/>
+      <c r="C48" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B49" s="4"/>
+      <c r="C49" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B50" s="4"/>
+      <c r="C50" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B51" s="4"/>
+      <c r="C51" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B52" s="4"/>
+      <c r="C52" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B53" s="4"/>
+      <c r="C53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B54" s="4"/>
+      <c r="C54" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B55" s="4"/>
+      <c r="C55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B56" s="5"/>
+      <c r="C56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B57" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B58" s="1"/>
+      <c r="C58" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B59" s="1"/>
+      <c r="C59" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B61" s="1"/>
+      <c r="C61" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B62" s="1"/>
+      <c r="C62" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B46:B56"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="B9:B20"/>
     <mergeCell ref="B21:B28"/>

</xml_diff>

<commit_message>
260127 DataBaseCol 열어져 있는 파일 삭제. 및 col 수정
</commit_message>
<xml_diff>
--- a/db/DataBaseCol.xlsx
+++ b/db/DataBaseCol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\SAP_Straffic260119\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF72AA2B-66C4-4263-8BF2-56DEEA436A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50299A04-30C9-4A71-9960-9126F2B8D45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{008F3ED9-E954-48A9-9E03-D39CBFFCB847}"/>
   </bookViews>
@@ -230,10 +230,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>insident</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>등록일자 Default Current_Timestamp</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -242,14 +238,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Insident ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Insident 제목</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>인시던트 발생 호선명</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -270,38 +258,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>insident_id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>user_name</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>insident_title</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>insident_line_name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">insident_station_id </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>insident_station_name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>insident_content</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>insident_status</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>user_id</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -314,10 +274,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>insident_comment</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>작성자 ID ( FK storage.user(user_id) )</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -326,10 +282,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>인시던트 ID ( FK storage.insident(insident_id) )</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>댓글 ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -432,6 +384,42 @@
   <si>
     <t>인시던트 상태 (1:계획되지 않음 2:해결중 3:완료 4:비활성화)</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>incident</t>
+  </si>
+  <si>
+    <t>incident_id</t>
+  </si>
+  <si>
+    <t>incident ID</t>
+  </si>
+  <si>
+    <t>incident_title</t>
+  </si>
+  <si>
+    <t>incident 제목</t>
+  </si>
+  <si>
+    <t>incident_line_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incident_station_id </t>
+  </si>
+  <si>
+    <t>incident_station_name</t>
+  </si>
+  <si>
+    <t>incident_content</t>
+  </si>
+  <si>
+    <t>incident_status</t>
+  </si>
+  <si>
+    <t>incident_comment</t>
+  </si>
+  <si>
+    <t>인시던트 ID ( FK storage.incident(incident_id) )</t>
   </si>
 </sst>
 </file>
@@ -882,7 +870,7 @@
   <dimension ref="B2:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1038,7 +1026,7 @@
     <row r="12" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B12" s="5"/>
       <c r="C12" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
@@ -1051,7 +1039,7 @@
     <row r="13" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B13" s="5"/>
       <c r="C13" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
@@ -1064,20 +1052,20 @@
     <row r="14" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B14" s="5"/>
       <c r="C14" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B15" s="5"/>
       <c r="C15" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
@@ -1090,7 +1078,7 @@
     <row r="16" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B16" s="5"/>
       <c r="C16" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
@@ -1103,7 +1091,7 @@
     <row r="17" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B17" s="5"/>
       <c r="C17" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
@@ -1116,7 +1104,7 @@
     <row r="18" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B18" s="5"/>
       <c r="C18" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
@@ -1129,7 +1117,7 @@
     <row r="19" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B19" s="5"/>
       <c r="C19" s="1" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
@@ -1142,7 +1130,7 @@
     <row r="20" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B20" s="5"/>
       <c r="C20" s="1" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
@@ -1154,7 +1142,7 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B21" s="5" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>30</v>
@@ -1211,7 +1199,7 @@
     <row r="25" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B25" s="5"/>
       <c r="C25" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1222,7 +1210,7 @@
     <row r="26" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B26" s="5"/>
       <c r="C26" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1233,7 +1221,7 @@
     <row r="27" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B27" s="5"/>
       <c r="C27" s="1" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1254,7 +1242,7 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B29" s="5" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>37</v>
@@ -1311,7 +1299,7 @@
     <row r="33" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B33" s="5"/>
       <c r="C33" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1322,7 +1310,7 @@
     <row r="34" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B34" s="5"/>
       <c r="C34" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1333,7 +1321,7 @@
     <row r="35" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B35" s="5"/>
       <c r="C35" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1370,7 +1358,7 @@
         <v>45</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>31</v>
@@ -1385,7 +1373,7 @@
     <row r="39" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B39" s="5"/>
       <c r="C39" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
@@ -1411,7 +1399,7 @@
     <row r="41" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B41" s="5"/>
       <c r="C41" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
@@ -1424,7 +1412,7 @@
     <row r="42" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B42" s="5"/>
       <c r="C42" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
@@ -1437,7 +1425,7 @@
     <row r="43" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B43" s="5"/>
       <c r="C43" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
@@ -1450,7 +1438,7 @@
     <row r="44" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B44" s="5"/>
       <c r="C44" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -1473,10 +1461,10 @@
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B46" s="2" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>31</v>
@@ -1485,135 +1473,135 @@
         <v>31</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B47" s="3"/>
       <c r="C47" s="1" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B48" s="3"/>
       <c r="C48" s="1" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B49" s="3"/>
       <c r="C49" s="1" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B50" s="3"/>
       <c r="C50" s="1" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B51" s="3"/>
       <c r="C51" s="1" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B52" s="3"/>
       <c r="C52" s="1" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B53" s="3"/>
       <c r="C53" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B54" s="3"/>
       <c r="C54" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B55" s="3"/>
       <c r="C55" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B56" s="4"/>
       <c r="C56" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B57" s="2" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>31</v>
@@ -1622,70 +1610,70 @@
         <v>31</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B58" s="3"/>
       <c r="C58" s="1" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B59" s="3"/>
       <c r="C59" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B60" s="3"/>
       <c r="C60" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B61" s="3"/>
       <c r="C61" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B62" s="4"/>
       <c r="C62" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
260129 SQL 및 데이터베이스 필드 추가 Incident.incident_severity field 추가(인시던트 심각도)
</commit_message>
<xml_diff>
--- a/db/DataBaseCol.xlsx
+++ b/db/DataBaseCol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\SAP_Straffic260119\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50299A04-30C9-4A71-9960-9126F2B8D45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8189E177-8CD2-4417-9F1F-5D47397C8764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{008F3ED9-E954-48A9-9E03-D39CBFFCB847}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{008F3ED9-E954-48A9-9E03-D39CBFFCB847}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="104">
   <si>
     <t>DB</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -382,10 +382,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>인시던트 상태 (1:계획되지 않음 2:해결중 3:완료 4:비활성화)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>incident</t>
   </si>
   <si>
@@ -420,6 +416,18 @@
   </si>
   <si>
     <t>인시던트 ID ( FK storage.incident(incident_id) )</t>
+  </si>
+  <si>
+    <t>incident_severity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인시던트 진행 상태 (1:계획되지 않음 2:해결중 3:완료 4:비활성화)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">인시던트 심각도 ( 1:Critical 2:Major 3:Minor ) </t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -867,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A039B4-B4EC-499B-B846-66B839DA3680}">
-  <dimension ref="B2:F62"/>
+  <dimension ref="B2:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M49" sqref="M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -880,7 +888,7 @@
     <col min="3" max="3" width="21.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.69921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.4">
@@ -1461,38 +1469,38 @@
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B46" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="D46" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B47" s="3"/>
       <c r="C47" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B48" s="3"/>
       <c r="C48" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -1503,7 +1511,7 @@
     <row r="49" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B49" s="3"/>
       <c r="C49" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
@@ -1516,7 +1524,7 @@
     <row r="50" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B50" s="3"/>
       <c r="C50" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -1527,7 +1535,7 @@
     <row r="51" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B51" s="3"/>
       <c r="C51" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -1538,148 +1546,161 @@
     <row r="52" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B52" s="3"/>
       <c r="C52" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B53" s="3"/>
       <c r="C53" s="1" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B54" s="3"/>
       <c r="C54" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
+      <c r="E54" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="F54" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B55" s="3"/>
       <c r="C55" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B56" s="3"/>
+      <c r="C56" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F55" s="1" t="s">
+      <c r="D56" s="1"/>
+      <c r="E56" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B56" s="4"/>
-      <c r="C56" s="1" t="s">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B57" s="4"/>
+      <c r="C57" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1" t="s">
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B57" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C57" s="1" t="s">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B58" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F57" s="1" t="s">
+      <c r="D58" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B58" s="3"/>
-      <c r="C58" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B59" s="3"/>
       <c r="C59" s="1" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B60" s="3"/>
       <c r="C60" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B61" s="3"/>
       <c r="C61" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B62" s="3"/>
+      <c r="C62" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1" t="s">
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B62" s="4"/>
-      <c r="C62" s="1" t="s">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B63" s="4"/>
+      <c r="C63" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F62" s="1" t="s">
+      <c r="D63" s="1"/>
+      <c r="E63" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B57:B62"/>
-    <mergeCell ref="B46:B56"/>
+    <mergeCell ref="B58:B63"/>
+    <mergeCell ref="B46:B57"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="B9:B20"/>
     <mergeCell ref="B21:B28"/>

</xml_diff>

<commit_message>
260129 local_amenities.csv Import 가능 파일로 만들기.
</commit_message>
<xml_diff>
--- a/db/DataBaseCol.xlsx
+++ b/db/DataBaseCol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\SAP_Straffic260119\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933DED3D-7061-47AE-8263-A6461F0EA283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C68AD9-70F1-4657-A55B-2339D93648FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{008F3ED9-E954-48A9-9E03-D39CBFFCB847}"/>
   </bookViews>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A039B4-B4EC-499B-B846-66B839DA3680}">
   <dimension ref="B2:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
260129 DataBaseCol 변경 계획되지않음 > 대기 로 변경  incident_status
</commit_message>
<xml_diff>
--- a/db/DataBaseCol.xlsx
+++ b/db/DataBaseCol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\SAP_Straffic260119\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C68AD9-70F1-4657-A55B-2339D93648FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04987EC-56DB-465D-9FD5-37DA728CC1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{008F3ED9-E954-48A9-9E03-D39CBFFCB847}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{008F3ED9-E954-48A9-9E03-D39CBFFCB847}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="104">
   <si>
     <t>DB</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -422,11 +422,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>인시던트 진행 상태 (1:계획되지 않음 2:해결중 3:완료 4:비활성화)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">인시던트 심각도 ( 1:Critical 2:Major 3:Minor ) </t>
+    <t>인시던트 진행 상태 (1:대기 2:해결중 3:완료 4:비활성화)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">인시던트 심각도(1:Critical 2:Major 3:Minor) </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A039B4-B4EC-499B-B846-66B839DA3680}">
   <dimension ref="B2:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J58" sqref="J58"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1560,9 +1560,7 @@
         <v>101</v>
       </c>
       <c r="D53" s="1"/>
-      <c r="E53" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
         <v>103</v>
       </c>

</xml_diff>